<commit_message>
Edit logic counting, Edit weights path
</commit_message>
<xml_diff>
--- a/vehicle_information.xlsx
+++ b/vehicle_information.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D262"/>
+  <dimension ref="A1:D300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5005,10 +5005,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D254" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D254" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="255">
@@ -5025,10 +5023,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D255" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D255" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="256">
@@ -5045,10 +5041,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D256" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D256" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="257">
@@ -5065,10 +5059,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D257" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D257" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -5085,10 +5077,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D258" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D258" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="259">
@@ -5105,10 +5095,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D259" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D259" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="260">
@@ -5125,10 +5113,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D260" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D260" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="261">
@@ -5145,10 +5131,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D261" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D261" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="262">
@@ -5165,9 +5149,767 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D262" t="inlineStr">
+      <c r="D262" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:41:24</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>2</v>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>31.51</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:41:25</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>4</v>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>45.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:41:25</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>5</v>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>41.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:41:31</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>9</v>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>41.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:41:33</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>10</v>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>51.41</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:41:34</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>13</v>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>41.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:41:36</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>14</v>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>42.43</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:08</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>25</v>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
         <is>
           <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:09</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>27</v>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:10</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>28</v>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:11</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>31</v>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:14</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>34</v>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:15</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>32</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:16</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>35</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:18</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>33</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:18</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>36</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:21</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>37</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:21</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>39</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:23</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>40</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:24</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>41</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:28</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>49</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>38.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:29</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>50</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>43.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:30</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>51</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>48.93</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:31</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>46</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>90.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:33</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>52</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>15.26</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:35</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>53</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>44.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:36</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>54</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>42.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:38</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>55</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>40.32</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:38</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>56</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>44.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:41</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>57</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>35.97</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:41</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>58</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>41.35</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:43</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>61</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>51.75</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:51</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>64</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>123.76</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:54</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>66</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>87.57</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:55</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>68</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>74.44</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:57</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>67</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>112.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:44:58</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>69</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>111.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2025-06-03 20:45:02</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>70</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Truck</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>19.27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add object detector selection feature
</commit_message>
<xml_diff>
--- a/vehicle_information.xlsx
+++ b/vehicle_information.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D300"/>
+  <dimension ref="A1:D370"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5167,10 +5167,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D263" t="inlineStr">
-        <is>
-          <t>31.51</t>
-        </is>
+      <c r="D263" t="n">
+        <v>31.51</v>
       </c>
     </row>
     <row r="264">
@@ -5187,10 +5185,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D264" t="inlineStr">
-        <is>
-          <t>45.77</t>
-        </is>
+      <c r="D264" t="n">
+        <v>45.77</v>
       </c>
     </row>
     <row r="265">
@@ -5207,10 +5203,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D265" t="inlineStr">
-        <is>
-          <t>41.46</t>
-        </is>
+      <c r="D265" t="n">
+        <v>41.46</v>
       </c>
     </row>
     <row r="266">
@@ -5227,10 +5221,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D266" t="inlineStr">
-        <is>
-          <t>41.01</t>
-        </is>
+      <c r="D266" t="n">
+        <v>41.01</v>
       </c>
     </row>
     <row r="267">
@@ -5247,10 +5239,8 @@
           <t>Truck</t>
         </is>
       </c>
-      <c r="D267" t="inlineStr">
-        <is>
-          <t>51.41</t>
-        </is>
+      <c r="D267" t="n">
+        <v>51.41</v>
       </c>
     </row>
     <row r="268">
@@ -5267,10 +5257,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D268" t="inlineStr">
-        <is>
-          <t>41.89</t>
-        </is>
+      <c r="D268" t="n">
+        <v>41.89</v>
       </c>
     </row>
     <row r="269">
@@ -5287,10 +5275,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D269" t="inlineStr">
-        <is>
-          <t>42.43</t>
-        </is>
+      <c r="D269" t="n">
+        <v>42.43</v>
       </c>
     </row>
     <row r="270">
@@ -5307,10 +5293,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D270" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D270" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -5327,10 +5311,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D271" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D271" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="272">
@@ -5347,10 +5329,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D272" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D272" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -5367,10 +5347,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D273" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D273" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="274">
@@ -5387,10 +5365,8 @@
           <t>Bus</t>
         </is>
       </c>
-      <c r="D274" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D274" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="275">
@@ -5407,10 +5383,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D275" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D275" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="276">
@@ -5427,10 +5401,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D276" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D276" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="277">
@@ -5447,10 +5419,8 @@
           <t>Truck</t>
         </is>
       </c>
-      <c r="D277" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D277" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="278">
@@ -5467,10 +5437,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D278" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D278" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="279">
@@ -5487,10 +5455,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D279" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D279" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="280">
@@ -5507,10 +5473,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D280" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D280" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="281">
@@ -5527,10 +5491,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D281" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D281" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="282">
@@ -5547,10 +5509,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D282" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
+      <c r="D282" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="283">
@@ -5567,10 +5527,8 @@
           <t>Truck</t>
         </is>
       </c>
-      <c r="D283" t="inlineStr">
-        <is>
-          <t>38.01</t>
-        </is>
+      <c r="D283" t="n">
+        <v>38.01</v>
       </c>
     </row>
     <row r="284">
@@ -5587,10 +5545,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D284" t="inlineStr">
-        <is>
-          <t>43.20</t>
-        </is>
+      <c r="D284" t="n">
+        <v>43.2</v>
       </c>
     </row>
     <row r="285">
@@ -5607,10 +5563,8 @@
           <t>Truck</t>
         </is>
       </c>
-      <c r="D285" t="inlineStr">
-        <is>
-          <t>48.93</t>
-        </is>
+      <c r="D285" t="n">
+        <v>48.93</v>
       </c>
     </row>
     <row r="286">
@@ -5627,10 +5581,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D286" t="inlineStr">
-        <is>
-          <t>90.28</t>
-        </is>
+      <c r="D286" t="n">
+        <v>90.28</v>
       </c>
     </row>
     <row r="287">
@@ -5647,10 +5599,8 @@
           <t>Bus</t>
         </is>
       </c>
-      <c r="D287" t="inlineStr">
-        <is>
-          <t>15.26</t>
-        </is>
+      <c r="D287" t="n">
+        <v>15.26</v>
       </c>
     </row>
     <row r="288">
@@ -5667,10 +5617,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D288" t="inlineStr">
-        <is>
-          <t>44.99</t>
-        </is>
+      <c r="D288" t="n">
+        <v>44.99</v>
       </c>
     </row>
     <row r="289">
@@ -5687,10 +5635,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D289" t="inlineStr">
-        <is>
-          <t>42.89</t>
-        </is>
+      <c r="D289" t="n">
+        <v>42.89</v>
       </c>
     </row>
     <row r="290">
@@ -5707,10 +5653,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D290" t="inlineStr">
-        <is>
-          <t>40.32</t>
-        </is>
+      <c r="D290" t="n">
+        <v>40.32</v>
       </c>
     </row>
     <row r="291">
@@ -5727,10 +5671,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D291" t="inlineStr">
-        <is>
-          <t>44.76</t>
-        </is>
+      <c r="D291" t="n">
+        <v>44.76</v>
       </c>
     </row>
     <row r="292">
@@ -5747,10 +5689,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D292" t="inlineStr">
-        <is>
-          <t>35.97</t>
-        </is>
+      <c r="D292" t="n">
+        <v>35.97</v>
       </c>
     </row>
     <row r="293">
@@ -5767,10 +5707,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D293" t="inlineStr">
-        <is>
-          <t>41.35</t>
-        </is>
+      <c r="D293" t="n">
+        <v>41.35</v>
       </c>
     </row>
     <row r="294">
@@ -5787,10 +5725,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D294" t="inlineStr">
-        <is>
-          <t>51.75</t>
-        </is>
+      <c r="D294" t="n">
+        <v>51.75</v>
       </c>
     </row>
     <row r="295">
@@ -5807,10 +5743,8 @@
           <t>Truck</t>
         </is>
       </c>
-      <c r="D295" t="inlineStr">
-        <is>
-          <t>123.76</t>
-        </is>
+      <c r="D295" t="n">
+        <v>123.76</v>
       </c>
     </row>
     <row r="296">
@@ -5827,10 +5761,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D296" t="inlineStr">
-        <is>
-          <t>87.57</t>
-        </is>
+      <c r="D296" t="n">
+        <v>87.56999999999999</v>
       </c>
     </row>
     <row r="297">
@@ -5847,10 +5779,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D297" t="inlineStr">
-        <is>
-          <t>74.44</t>
-        </is>
+      <c r="D297" t="n">
+        <v>74.44</v>
       </c>
     </row>
     <row r="298">
@@ -5867,10 +5797,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D298" t="inlineStr">
-        <is>
-          <t>112.09</t>
-        </is>
+      <c r="D298" t="n">
+        <v>112.09</v>
       </c>
     </row>
     <row r="299">
@@ -5887,10 +5815,8 @@
           <t>Car</t>
         </is>
       </c>
-      <c r="D299" t="inlineStr">
-        <is>
-          <t>111.01</t>
-        </is>
+      <c r="D299" t="n">
+        <v>111.01</v>
       </c>
     </row>
     <row r="300">
@@ -5907,9 +5833,1015 @@
           <t>Truck</t>
         </is>
       </c>
-      <c r="D300" t="inlineStr">
-        <is>
-          <t>19.27</t>
+      <c r="D300" t="n">
+        <v>19.27</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:32</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>2</v>
+      </c>
+      <c r="C301" t="inlineStr"/>
+      <c r="D301" t="n">
+        <v>31.51</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:32</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>4</v>
+      </c>
+      <c r="C302" t="inlineStr"/>
+      <c r="D302" t="n">
+        <v>45.77</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:33</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>5</v>
+      </c>
+      <c r="C303" t="inlineStr"/>
+      <c r="D303" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:34</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>8</v>
+      </c>
+      <c r="C304" t="inlineStr"/>
+      <c r="D304" t="n">
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:38</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>11</v>
+      </c>
+      <c r="C305" t="inlineStr"/>
+      <c r="D305" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:39</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>9</v>
+      </c>
+      <c r="C306" t="inlineStr"/>
+      <c r="D306" t="n">
+        <v>41.01</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:39</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>12</v>
+      </c>
+      <c r="C307" t="inlineStr"/>
+      <c r="D307" t="n">
+        <v>18.09</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:41</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>10</v>
+      </c>
+      <c r="C308" t="inlineStr"/>
+      <c r="D308" t="n">
+        <v>51.41</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:42</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>13</v>
+      </c>
+      <c r="C309" t="inlineStr"/>
+      <c r="D309" t="n">
+        <v>41.89</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:45</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>14</v>
+      </c>
+      <c r="C310" t="inlineStr"/>
+      <c r="D310" t="n">
+        <v>42.43</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:45</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>16</v>
+      </c>
+      <c r="C311" t="inlineStr"/>
+      <c r="D311" t="n">
+        <v>17.84</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:25:47</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>17</v>
+      </c>
+      <c r="C312" t="inlineStr"/>
+      <c r="D312" t="n">
+        <v>17.59</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:32:03</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>2</v>
+      </c>
+      <c r="C313" t="inlineStr"/>
+      <c r="D313" t="n">
+        <v>31.51</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:32:04</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>4</v>
+      </c>
+      <c r="C314" t="inlineStr"/>
+      <c r="D314" t="n">
+        <v>45.77</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:32:05</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>5</v>
+      </c>
+      <c r="C315" t="inlineStr"/>
+      <c r="D315" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:32:19</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>12</v>
+      </c>
+      <c r="C316" t="inlineStr"/>
+      <c r="D316" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:32:20</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>14</v>
+      </c>
+      <c r="C317" t="inlineStr"/>
+      <c r="D317" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:32:21</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>15</v>
+      </c>
+      <c r="C318" t="inlineStr"/>
+      <c r="D318" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>2025-06-03 22:32:22</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>18</v>
+      </c>
+      <c r="C319" t="inlineStr"/>
+      <c r="D319" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:31:58</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>2</v>
+      </c>
+      <c r="C320" t="inlineStr"/>
+      <c r="D320" t="n">
+        <v>31.51</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:31:59</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>4</v>
+      </c>
+      <c r="C321" t="inlineStr"/>
+      <c r="D321" t="n">
+        <v>45.77</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:00</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>5</v>
+      </c>
+      <c r="C322" t="inlineStr"/>
+      <c r="D322" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:01</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>8</v>
+      </c>
+      <c r="C323" t="inlineStr"/>
+      <c r="D323" t="n">
+        <v>18.28</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:12</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>11</v>
+      </c>
+      <c r="C324" t="inlineStr"/>
+      <c r="D324" t="n">
+        <v>27.01</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:15</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>12</v>
+      </c>
+      <c r="C325" t="inlineStr"/>
+      <c r="D325" t="n">
+        <v>33.04</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:19</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>17</v>
+      </c>
+      <c r="C326" t="inlineStr"/>
+      <c r="D326" t="n">
+        <v>40.92</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:25</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>14</v>
+      </c>
+      <c r="C327" t="inlineStr"/>
+      <c r="D327" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:38</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>30</v>
+      </c>
+      <c r="C328" t="inlineStr"/>
+      <c r="D328" t="n">
+        <v>17.16</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:39</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>36</v>
+      </c>
+      <c r="C329" t="inlineStr"/>
+      <c r="D329" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:44</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>19</v>
+      </c>
+      <c r="C330" t="inlineStr"/>
+      <c r="D330" t="n">
+        <v>41.03</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:47</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>33</v>
+      </c>
+      <c r="C331" t="inlineStr"/>
+      <c r="D331" t="n">
+        <v>18.09</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:54</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>20</v>
+      </c>
+      <c r="C332" t="inlineStr"/>
+      <c r="D332" t="n">
+        <v>58.54</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:32:59</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>26</v>
+      </c>
+      <c r="C333" t="inlineStr"/>
+      <c r="D333" t="n">
+        <v>41.8</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:09</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>32</v>
+      </c>
+      <c r="C334" t="inlineStr"/>
+      <c r="D334" t="n">
+        <v>42.34</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:09</t>
+        </is>
+      </c>
+      <c r="B335" t="n">
+        <v>37</v>
+      </c>
+      <c r="C335" t="inlineStr"/>
+      <c r="D335" t="n">
+        <v>18.01</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:19</t>
+        </is>
+      </c>
+      <c r="B336" t="n">
+        <v>39</v>
+      </c>
+      <c r="C336" t="inlineStr"/>
+      <c r="D336" t="n">
+        <v>17.52</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:24</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>35</v>
+      </c>
+      <c r="C337" t="inlineStr"/>
+      <c r="D337" t="n">
+        <v>34.66</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:35</t>
+        </is>
+      </c>
+      <c r="B338" t="n">
+        <v>41</v>
+      </c>
+      <c r="C338" t="inlineStr"/>
+      <c r="D338" t="n">
+        <v>19.11</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:45</t>
+        </is>
+      </c>
+      <c r="B339" t="n">
+        <v>38</v>
+      </c>
+      <c r="C339" t="inlineStr"/>
+      <c r="D339" t="n">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:45</t>
+        </is>
+      </c>
+      <c r="B340" t="n">
+        <v>43</v>
+      </c>
+      <c r="C340" t="inlineStr"/>
+      <c r="D340" t="n">
+        <v>16.67</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:33:52</t>
+        </is>
+      </c>
+      <c r="B341" t="n">
+        <v>45</v>
+      </c>
+      <c r="C341" t="inlineStr"/>
+      <c r="D341" t="n">
+        <v>16.91</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:34:03</t>
+        </is>
+      </c>
+      <c r="B342" t="n">
+        <v>40</v>
+      </c>
+      <c r="C342" t="inlineStr"/>
+      <c r="D342" t="n">
+        <v>34.7</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:34:23</t>
+        </is>
+      </c>
+      <c r="B343" t="n">
+        <v>47</v>
+      </c>
+      <c r="C343" t="inlineStr"/>
+      <c r="D343" t="n">
+        <v>17.73</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:34:30</t>
+        </is>
+      </c>
+      <c r="B344" t="n">
+        <v>48</v>
+      </c>
+      <c r="C344" t="inlineStr"/>
+      <c r="D344" t="n">
+        <v>16.66</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:34:37</t>
+        </is>
+      </c>
+      <c r="B345" t="n">
+        <v>51</v>
+      </c>
+      <c r="C345" t="inlineStr"/>
+      <c r="D345" t="n">
+        <v>18.1</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:34:56</t>
+        </is>
+      </c>
+      <c r="B346" t="n">
+        <v>49</v>
+      </c>
+      <c r="C346" t="inlineStr"/>
+      <c r="D346" t="n">
+        <v>39.92</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:35:04</t>
+        </is>
+      </c>
+      <c r="B347" t="n">
+        <v>55</v>
+      </c>
+      <c r="C347" t="inlineStr"/>
+      <c r="D347" t="n">
+        <v>17.32</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:35:09</t>
+        </is>
+      </c>
+      <c r="B348" t="n">
+        <v>56</v>
+      </c>
+      <c r="C348" t="inlineStr"/>
+      <c r="D348" t="n">
+        <v>19.23</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:35:11</t>
+        </is>
+      </c>
+      <c r="B349" t="n">
+        <v>57</v>
+      </c>
+      <c r="C349" t="inlineStr"/>
+      <c r="D349" t="n">
+        <v>18.45</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:35:17</t>
+        </is>
+      </c>
+      <c r="B350" t="n">
+        <v>52</v>
+      </c>
+      <c r="C350" t="inlineStr"/>
+      <c r="D350" t="n">
+        <v>38.61</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:35:40</t>
+        </is>
+      </c>
+      <c r="B351" t="n">
+        <v>61</v>
+      </c>
+      <c r="C351" t="inlineStr"/>
+      <c r="D351" t="n">
+        <v>17.17</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:35:40</t>
+        </is>
+      </c>
+      <c r="B352" t="n">
+        <v>62</v>
+      </c>
+      <c r="C352" t="inlineStr"/>
+      <c r="D352" t="n">
+        <v>19.11</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:35:51</t>
+        </is>
+      </c>
+      <c r="B353" t="n">
+        <v>67</v>
+      </c>
+      <c r="C353" t="inlineStr"/>
+      <c r="D353" t="n">
+        <v>17.04</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:36:00</t>
+        </is>
+      </c>
+      <c r="B354" t="n">
+        <v>72</v>
+      </c>
+      <c r="C354" t="inlineStr"/>
+      <c r="D354" t="n">
+        <v>18.46</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:36:06</t>
+        </is>
+      </c>
+      <c r="B355" t="n">
+        <v>58</v>
+      </c>
+      <c r="C355" t="inlineStr"/>
+      <c r="D355" t="n">
+        <v>35.4</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:36:07</t>
+        </is>
+      </c>
+      <c r="B356" t="n">
+        <v>53</v>
+      </c>
+      <c r="C356" t="inlineStr"/>
+      <c r="D356" t="n">
+        <v>40.68</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:56:35</t>
+        </is>
+      </c>
+      <c r="B357" t="n">
+        <v>2</v>
+      </c>
+      <c r="C357" t="inlineStr"/>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>31.51</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:56:36</t>
+        </is>
+      </c>
+      <c r="B358" t="n">
+        <v>4</v>
+      </c>
+      <c r="C358" t="inlineStr"/>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>45.77</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:56:37</t>
+        </is>
+      </c>
+      <c r="B359" t="n">
+        <v>5</v>
+      </c>
+      <c r="C359" t="inlineStr"/>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>41.46</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:56:38</t>
+        </is>
+      </c>
+      <c r="B360" t="n">
+        <v>8</v>
+      </c>
+      <c r="C360" t="inlineStr"/>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>18.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:56:58</t>
+        </is>
+      </c>
+      <c r="B361" t="n">
+        <v>14</v>
+      </c>
+      <c r="C361" t="inlineStr"/>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>27.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:02</t>
+        </is>
+      </c>
+      <c r="B362" t="n">
+        <v>15</v>
+      </c>
+      <c r="C362" t="inlineStr"/>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>33.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:05</t>
+        </is>
+      </c>
+      <c r="B363" t="n">
+        <v>20</v>
+      </c>
+      <c r="C363" t="inlineStr"/>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>40.92</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:30</t>
+        </is>
+      </c>
+      <c r="B364" t="n">
+        <v>36</v>
+      </c>
+      <c r="C364" t="inlineStr"/>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>31.51</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:31</t>
+        </is>
+      </c>
+      <c r="B365" t="n">
+        <v>39</v>
+      </c>
+      <c r="C365" t="inlineStr"/>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>41.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:32</t>
+        </is>
+      </c>
+      <c r="B366" t="n">
+        <v>40</v>
+      </c>
+      <c r="C366" t="inlineStr"/>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>18.28</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:35</t>
+        </is>
+      </c>
+      <c r="B367" t="n">
+        <v>43</v>
+      </c>
+      <c r="C367" t="inlineStr"/>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>19.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:36</t>
+        </is>
+      </c>
+      <c r="B368" t="n">
+        <v>45</v>
+      </c>
+      <c r="C368" t="inlineStr"/>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>42.31</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:57:37</t>
+        </is>
+      </c>
+      <c r="B369" t="n">
+        <v>46</v>
+      </c>
+      <c r="C369" t="inlineStr"/>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>17.96</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>2025-06-03 23:58:36</t>
+        </is>
+      </c>
+      <c r="B370" t="n">
+        <v>49</v>
+      </c>
+      <c r="C370" t="inlineStr"/>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>27.01</t>
         </is>
       </c>
     </row>

</xml_diff>